<commit_message>
últimos cambios en el código y medición de tiempos
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p7/P7_UO277876.xlsx
+++ b/src/main/java/algestudiante/p7/P7_UO277876.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAC24E0-4B31-439C-8AEF-2A89299D7246}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97739C2-4DD0-44A7-8209-14933ED0A209}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9444" yWindow="768" windowWidth="10764" windowHeight="9480" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Ramifica y poda" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>nVeces</t>
   </si>
@@ -54,18 +54,6 @@
     <t>Complejidad:</t>
   </si>
   <si>
-    <t>nVeces = 100</t>
-  </si>
-  <si>
-    <t>nVeces = 10000</t>
-  </si>
-  <si>
-    <t>nVeces = 1000</t>
-  </si>
-  <si>
-    <t>Me para en 15</t>
-  </si>
-  <si>
     <t>t(ryp)</t>
   </si>
   <si>
@@ -73,6 +61,9 @@
   </si>
   <si>
     <t>O(3^n)</t>
+  </si>
+  <si>
+    <t>nVeces = 1000000</t>
   </si>
 </sst>
 </file>
@@ -267,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -302,7 +293,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,36 +418,138 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ramifica y poda'!$A$3:$A$5</c:f>
+              <c:f>'Ramifica y poda'!$A$3:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>204800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>409600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>819200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1638400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3276800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6553600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13107200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26214400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52428800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ramifica y poda'!$B$3:$B$5</c:f>
+              <c:f>'Ramifica y poda'!$B$3:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.3299999999999999E-2</c:v>
+                  <c:v>1.97E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0819999999999999</c:v>
+                  <c:v>1.8649999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>525.6</c:v>
+                  <c:v>1.377E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0800000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3399999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.109E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0970000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.709E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1980000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7409999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.152E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0300000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9650000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.1400000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4910000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.902E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.8600000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.645E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.477E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.9740000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,16 +1308,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1552,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50AC779-C55D-4822-8A6D-58AA05F2A758}">
-  <dimension ref="A2:I22"/>
+  <dimension ref="A2:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1574,10 +1666,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>1</v>
@@ -1589,14 +1681,14 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="B3" s="17">
-        <f>133/I8</f>
-        <v>1.3299999999999999E-2</v>
+        <f>1970/I6</f>
+        <v>1.97E-3</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>2</v>
@@ -1608,15 +1700,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="B4" s="17">
-        <f>2082/I9</f>
-        <v>2.0819999999999999</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>8</v>
-      </c>
+        <f>1865/I6</f>
+        <v>1.8649999999999999E-3</v>
+      </c>
+      <c r="C4" s="7"/>
       <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1627,99 +1717,215 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
-        <v>15</v>
+        <v>400</v>
       </c>
       <c r="B5" s="17">
-        <f>52560/I10</f>
-        <v>525.6</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>6</v>
-      </c>
+        <f>1377/I6</f>
+        <v>1.377E-3</v>
+      </c>
+      <c r="C5" s="7"/>
       <c r="I5" s="2">
         <v>10000000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
-        <v>20</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="20"/>
+      <c r="A6" s="15">
+        <v>800</v>
+      </c>
+      <c r="B6" s="17">
+        <f>608/I6</f>
+        <v>6.0800000000000003E-4</v>
+      </c>
+      <c r="C6" s="7"/>
       <c r="I6" s="2">
         <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="15">
+        <v>1600</v>
+      </c>
+      <c r="B7" s="17">
+        <f>534/I6</f>
+        <v>5.3399999999999997E-4</v>
+      </c>
+      <c r="C7" s="7"/>
       <c r="I7" s="3">
         <v>100000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>3200</v>
+      </c>
+      <c r="B8" s="17">
+        <f>1109/I6</f>
+        <v>1.109E-3</v>
+      </c>
+      <c r="C8" s="7"/>
       <c r="I8" s="2">
         <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>6400</v>
+      </c>
+      <c r="B9" s="17">
+        <f>1097/I6</f>
+        <v>1.0970000000000001E-3</v>
+      </c>
+      <c r="C9" s="7"/>
       <c r="I9" s="13">
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+      <c r="A10" s="15">
+        <v>12800</v>
+      </c>
+      <c r="B10" s="17">
+        <f>1709/I6</f>
+        <v>1.709E-3</v>
+      </c>
+      <c r="C10" s="7"/>
       <c r="I10" s="13">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+      <c r="A11" s="15">
+        <v>25600</v>
+      </c>
+      <c r="B11" s="17">
+        <f>1198/I6</f>
+        <v>1.1980000000000001E-3</v>
+      </c>
+      <c r="C11" s="7"/>
       <c r="I11" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+      <c r="A12" s="15">
+        <v>51200</v>
+      </c>
+      <c r="B12" s="17">
+        <f>1741/I6</f>
+        <v>1.7409999999999999E-3</v>
+      </c>
+      <c r="C12" s="7"/>
       <c r="I12" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
+      <c r="A13" s="15">
+        <v>102400</v>
+      </c>
+      <c r="B13" s="17">
+        <f>1152/I6</f>
+        <v>1.152E-3</v>
+      </c>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="15">
+        <v>204800</v>
+      </c>
+      <c r="B14" s="17">
+        <f>603/I6</f>
+        <v>6.0300000000000002E-4</v>
+      </c>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
+      <c r="A15" s="15">
+        <v>409600</v>
+      </c>
+      <c r="B15" s="17">
+        <f>1965/I6</f>
+        <v>1.9650000000000002E-3</v>
+      </c>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
+      <c r="A16" s="15">
+        <v>819200</v>
+      </c>
+      <c r="B16" s="17">
+        <f>714/I6</f>
+        <v>7.1400000000000001E-4</v>
+      </c>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="15">
+        <v>1638400</v>
+      </c>
+      <c r="B17" s="17">
+        <f>2491/I6</f>
+        <v>2.4910000000000002E-3</v>
+      </c>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
+        <v>3276800</v>
+      </c>
+      <c r="B18" s="17">
+        <f>1902/I6</f>
+        <v>1.902E-3</v>
+      </c>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
+        <v>6553600</v>
+      </c>
+      <c r="B19" s="17">
+        <f>2860/I6</f>
+        <v>2.8600000000000001E-3</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
+        <v>13107200</v>
+      </c>
+      <c r="B20" s="17">
+        <f>1645/I6</f>
+        <v>1.645E-3</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
+        <v>26214400</v>
+      </c>
+      <c r="B21" s="17">
+        <f>1477/I6</f>
+        <v>1.477E-3</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>52428800</v>
+      </c>
+      <c r="B22" s="19">
+        <f>3974/I6</f>
+        <v>3.9740000000000001E-3</v>
+      </c>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>